<commit_message>
Added Textwrapping and Numberformatting on MainMetro, Edited excel templates for better look and easier reading
</commit_message>
<xml_diff>
--- a/Stockbook/Stockbook/Invoice Template.xlsx
+++ b/Stockbook/Stockbook/Invoice Template.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franz Justin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Source\Repos\Stockbook\Stockbook\Stockbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14952" windowHeight="5688"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14950" windowHeight="5690"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>Northern Ventures</t>
-  </si>
-  <si>
     <t xml:space="preserve">SALES INVOICE - REFERENCE NUMBER </t>
   </si>
   <si>
@@ -50,15 +47,9 @@
     <t>DISCOUNT:</t>
   </si>
   <si>
-    <t>TERR CODE</t>
-  </si>
-  <si>
     <t>UOM</t>
   </si>
   <si>
-    <t>QUANTITY SERVES</t>
-  </si>
-  <si>
     <t>UNIT PRICE</t>
   </si>
   <si>
@@ -66,6 +57,17 @@
   </si>
   <si>
     <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>PODUCT 
+CODE</t>
+  </si>
+  <si>
+    <t>QUANTITY
+ SERVES</t>
+  </si>
+  <si>
+    <t>Change Name of the Company in Settings</t>
   </si>
 </sst>
 </file>
@@ -147,20 +149,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -479,108 +492,114 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="9.77734375" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="9.77734375" customWidth="1"/>
+    <col min="1" max="1" width="9.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.08984375" customWidth="1"/>
+    <col min="7" max="10" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="6" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="G5" s="8"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="6" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="24.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="D8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -592,7 +611,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -604,19 +623,19 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="5"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -628,17 +647,15 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="27" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="13.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="6">
+    <mergeCell ref="A6:E6"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:F3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>